<commit_message>
Implementacao das chaves estrangeiras FK
</commit_message>
<xml_diff>
--- a/DATABASE/MASSA_DE_DADOS_SQN.xlsx
+++ b/DATABASE/MASSA_DE_DADOS_SQN.xlsx
@@ -329,6 +329,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -336,9 +339,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,15 +698,15 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -820,17 +820,17 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="12"/>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -936,17 +936,17 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1078,17 +1078,17 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -1253,19 +1253,19 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="12"/>
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1379,10 +1379,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="11"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -1401,10 +1401,10 @@
         <v>58</v>
       </c>
       <c r="D39" s="2"/>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="12"/>
+      <c r="F39" s="9"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -1553,15 +1553,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="B23:D23"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B15:J15"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="F32:J32"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="B23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Lista de consultas para entrega
</commit_message>
<xml_diff>
--- a/DATABASE/MASSA_DE_DADOS_SQN.xlsx
+++ b/DATABASE/MASSA_DE_DADOS_SQN.xlsx
@@ -54,9 +54,6 @@
     <t>DESPESA</t>
   </si>
   <si>
-    <t>CATEGORIAS</t>
-  </si>
-  <si>
     <t>SUBCATEGORIAS</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>US_CONTA</t>
   </si>
   <si>
-    <t>COD_US_ADM</t>
-  </si>
-  <si>
     <t>FORMA_PGTO</t>
   </si>
   <si>
@@ -199,6 +193,12 @@
   </si>
   <si>
     <t>DESCR_FORMA_PAGTO</t>
+  </si>
+  <si>
+    <t>COD_US_GRUPO</t>
+  </si>
+  <si>
+    <t>CATEGORIA</t>
   </si>
 </sst>
 </file>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,13 +726,13 @@
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -744,13 +744,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1">
         <v>1234</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
@@ -771,13 +771,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="6">
         <v>4321</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="6">
         <v>1</v>
@@ -851,16 +851,16 @@
         <v>9</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -879,10 +879,10 @@
         <v>4</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="5">
         <v>3687</v>
@@ -952,7 +952,7 @@
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>1</v>
@@ -967,16 +967,16 @@
         <v>9</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K16" s="2"/>
     </row>
@@ -995,10 +995,10 @@
         <v>3</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H17" s="5">
         <v>80</v>
@@ -1079,13 +1079,13 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="9" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="2"/>
       <c r="F23" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -1099,10 +1099,10 @@
         <v>8</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="6" t="s">
@@ -1112,7 +1112,7 @@
         <v>8</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1127,7 +1127,7 @@
         <v>11</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="6">
@@ -1137,7 +1137,7 @@
         <v>3</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1152,7 +1152,7 @@
         <v>11</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="6">
@@ -1162,7 +1162,7 @@
         <v>3</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1177,7 +1177,7 @@
         <v>11</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="6">
@@ -1187,7 +1187,7 @@
         <v>3</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1202,7 +1202,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="6"/>
@@ -1254,13 +1254,13 @@
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="12"/>
       <c r="E32" s="2"/>
       <c r="F32" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
@@ -1271,29 +1271,29 @@
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I33" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G33" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H33" s="6" t="s">
+      <c r="J33" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="K33" s="2"/>
     </row>
@@ -1303,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" s="6">
         <v>1</v>
@@ -1332,7 +1332,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D35" s="6">
         <v>3.8547899999999999</v>
@@ -1351,7 +1351,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" s="6">
         <v>4.3301600000000002</v>
@@ -1380,7 +1380,7 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="2"/>
@@ -1395,14 +1395,14 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="2"/>
@@ -1417,14 +1417,14 @@
         <v>1</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -1438,14 +1438,14 @@
         <v>2</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="6">
         <v>1</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -1459,14 +1459,14 @@
         <v>3</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="6">
         <v>2</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -1483,7 +1483,7 @@
         <v>3</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -1500,7 +1500,7 @@
         <v>4</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -1517,7 +1517,7 @@
         <v>5</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>

</xml_diff>